<commit_message>
render N+3 data and doc
</commit_message>
<xml_diff>
--- a/data-export/export_202112/macro-sum-nplus3.xlsx
+++ b/data-export/export_202112/macro-sum-nplus3.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P103"/>
+  <dimension ref="A1:P104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -464,10 +464,10 @@
         </is>
       </c>
       <c r="F2">
-        <v>428817212.1486667</v>
+        <v>198438759.942</v>
       </c>
       <c r="G2">
-        <v>175559708.924</v>
+        <v>83456169.07066667</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -485,16 +485,16 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>253257503.2246667</v>
+        <v>114982590.8713333</v>
       </c>
       <c r="N2">
-        <v>-4.866160452365875e-09</v>
+        <v>-4.012448092301687e-09</v>
       </c>
       <c r="O2">
-        <v>253257503.2246667</v>
+        <v>114982590.8713333</v>
       </c>
       <c r="P2">
-        <v>428817212.1486667</v>
+        <v>198438759.942</v>
       </c>
     </row>
     <row r="3">
@@ -522,10 +522,10 @@
         </is>
       </c>
       <c r="F3">
-        <v>640946254.3650174</v>
+        <v>442497116.2927836</v>
       </c>
       <c r="G3">
-        <v>354373640.872</v>
+        <v>242908139.8266667</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -543,16 +543,16 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>286572613.4930174</v>
+        <v>199588976.4661169</v>
       </c>
       <c r="N3">
-        <v>-1.008932789166768e-08</v>
+        <v>-3.321717182795207e-09</v>
       </c>
       <c r="O3">
-        <v>286572613.4930174</v>
+        <v>199588976.4661169</v>
       </c>
       <c r="P3">
-        <v>640946254.3650174</v>
+        <v>442497116.2927836</v>
       </c>
     </row>
     <row r="4">
@@ -580,16 +580,16 @@
         </is>
       </c>
       <c r="F4">
-        <v>5068623696.51</v>
+        <v>3251018874.488667</v>
       </c>
       <c r="G4">
-        <v>1991089923.936667</v>
+        <v>1279106190.607333</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>273155</v>
+        <v>163893</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -601,16 +601,16 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>3077260617.573333</v>
+        <v>1971748790.881333</v>
       </c>
       <c r="N4">
-        <v>273154.9999999964</v>
+        <v>163893.0000000031</v>
       </c>
       <c r="O4">
-        <v>3077533772.573333</v>
+        <v>1971912683.881333</v>
       </c>
       <c r="P4">
-        <v>5068623696.51</v>
+        <v>3251018874.488667</v>
       </c>
     </row>
     <row r="5">
@@ -633,10 +633,10 @@
         </is>
       </c>
       <c r="F5">
-        <v>4940375016.644667</v>
+        <v>3083768944.075333</v>
       </c>
       <c r="G5">
-        <v>2052757311.46</v>
+        <v>1302066961.502667</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -654,16 +654,16 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <v>2887617705.184667</v>
+        <v>1781701982.572667</v>
       </c>
       <c r="N5">
-        <v>1.678902966280778e-08</v>
+        <v>2.605762953559558e-09</v>
       </c>
       <c r="O5">
-        <v>2887617705.184667</v>
+        <v>1781701982.572667</v>
       </c>
       <c r="P5">
-        <v>4940375016.644667</v>
+        <v>3083768944.075333</v>
       </c>
     </row>
     <row r="6">
@@ -691,16 +691,16 @@
         </is>
       </c>
       <c r="F6">
-        <v>2758696.01</v>
+        <v>919565.3366666666</v>
       </c>
       <c r="G6">
-        <v>2069022.01</v>
+        <v>689674.0033333333</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>1225872.5</v>
+        <v>408624.1666666666</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -712,16 +712,16 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>689674</v>
+        <v>229891.3333333333</v>
       </c>
       <c r="N6">
-        <v>-2.328306436538696e-10</v>
+        <v>-7.761021455128987e-11</v>
       </c>
       <c r="O6">
-        <v>689673.9999999998</v>
+        <v>229891.3333333333</v>
       </c>
       <c r="P6">
-        <v>2758696.01</v>
+        <v>919565.3366666666</v>
       </c>
     </row>
     <row r="7">
@@ -749,10 +749,10 @@
         </is>
       </c>
       <c r="F7">
-        <v>648491449.6233333</v>
+        <v>427921271.6886666</v>
       </c>
       <c r="G7">
-        <v>281627077.2233333</v>
+        <v>187646461.9873333</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -770,16 +770,16 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>366864372.4</v>
+        <v>240274809.7013333</v>
       </c>
       <c r="N7">
-        <v>2.522331972916921e-10</v>
+        <v>3.492459654808046e-11</v>
       </c>
       <c r="O7">
-        <v>366864372.4</v>
+        <v>240274809.7013333</v>
       </c>
       <c r="P7">
-        <v>648491449.6233333</v>
+        <v>427921271.6886666</v>
       </c>
     </row>
     <row r="8">
@@ -802,10 +802,10 @@
         </is>
       </c>
       <c r="F8">
-        <v>222132552.676</v>
+        <v>138887666.6546667</v>
       </c>
       <c r="G8">
-        <v>99278005.73133333</v>
+        <v>62080374.57666667</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -823,16 +823,16 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <v>122854546.9446667</v>
+        <v>76807292.07799999</v>
       </c>
       <c r="N8">
-        <v>6.480452915032704e-10</v>
+        <v>6.014791627724966e-10</v>
       </c>
       <c r="O8">
-        <v>122854546.9446667</v>
+        <v>76807292.07800001</v>
       </c>
       <c r="P8">
-        <v>222132552.676</v>
+        <v>138887666.6546667</v>
       </c>
     </row>
     <row r="9">
@@ -860,10 +860,10 @@
         </is>
       </c>
       <c r="F9">
-        <v>97513518.28666666</v>
+        <v>82690003.65599999</v>
       </c>
       <c r="G9">
-        <v>50868118.54333333</v>
+        <v>42973559.42999999</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -881,16 +881,16 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <v>46645399.74333333</v>
+        <v>39716444.226</v>
       </c>
       <c r="N9">
-        <v>1.008932789166768e-09</v>
+        <v>-2.017865578333537e-10</v>
       </c>
       <c r="O9">
-        <v>46645399.74333333</v>
+        <v>39716444.226</v>
       </c>
       <c r="P9">
-        <v>97513518.28666666</v>
+        <v>82690003.65599999</v>
       </c>
     </row>
     <row r="10">
@@ -918,10 +918,10 @@
         </is>
       </c>
       <c r="F10">
-        <v>1570369826.012667</v>
+        <v>1185751454.615333</v>
       </c>
       <c r="G10">
-        <v>623975031.2146666</v>
+        <v>477045100.2666667</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -939,16 +939,16 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <v>946394794.798</v>
+        <v>708706354.3486667</v>
       </c>
       <c r="N10">
-        <v>1.024842883149783e-08</v>
+        <v>8.339217553536098e-09</v>
       </c>
       <c r="O10">
-        <v>946394794.798</v>
+        <v>708706354.3486667</v>
       </c>
       <c r="P10">
-        <v>1570369826.012667</v>
+        <v>1185751454.615333</v>
       </c>
     </row>
     <row r="11">
@@ -971,10 +971,10 @@
         </is>
       </c>
       <c r="F11">
-        <v>211020144.47</v>
+        <v>161908376.6286667</v>
       </c>
       <c r="G11">
-        <v>92425014.42999999</v>
+        <v>69306920.84866667</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -992,16 +992,16 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <v>118595130.04</v>
+        <v>92601455.78</v>
       </c>
       <c r="N11">
-        <v>-1.241763432820638e-09</v>
+        <v>-3.073364496231079e-09</v>
       </c>
       <c r="O11">
-        <v>118595130.04</v>
+        <v>92601455.78</v>
       </c>
       <c r="P11">
-        <v>211020144.47</v>
+        <v>161908376.6286667</v>
       </c>
     </row>
     <row r="12">
@@ -1029,10 +1029,10 @@
         </is>
       </c>
       <c r="F12">
-        <v>259451344.3093333</v>
+        <v>182311578.72</v>
       </c>
       <c r="G12">
-        <v>139925942.2333333</v>
+        <v>97766171.45866667</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1041,7 +1041,7 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>37071233.89533333</v>
+        <v>35563521.62866667</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -1050,16 +1050,16 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <v>82454168.18066667</v>
+        <v>48981885.63266666</v>
       </c>
       <c r="N12">
-        <v>37071233.89533332</v>
+        <v>35563521.62866666</v>
       </c>
       <c r="O12">
-        <v>119525402.076</v>
+        <v>84545407.26133333</v>
       </c>
       <c r="P12">
-        <v>259451344.3093333</v>
+        <v>182311578.72</v>
       </c>
     </row>
     <row r="13">
@@ -1087,10 +1087,10 @@
         </is>
       </c>
       <c r="F13">
-        <v>1317136940.224</v>
+        <v>859217424.1159999</v>
       </c>
       <c r="G13">
-        <v>588406670.6966667</v>
+        <v>387817891.7473333</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1105,19 +1105,19 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>19943100.00333333</v>
+        <v>7366433.336666666</v>
       </c>
       <c r="M13">
-        <v>727652169.524</v>
+        <v>470321432.3653333</v>
       </c>
       <c r="N13">
         <v>1078100.003333332</v>
       </c>
       <c r="O13">
-        <v>728730269.5273334</v>
+        <v>471399532.3686666</v>
       </c>
       <c r="P13">
-        <v>1317136940.224</v>
+        <v>859217424.1159999</v>
       </c>
     </row>
     <row r="14">
@@ -1145,10 +1145,10 @@
         </is>
       </c>
       <c r="F14">
-        <v>82686595.53333333</v>
+        <v>58726423.428</v>
       </c>
       <c r="G14">
-        <v>65273148.84933333</v>
+        <v>46304550.18266667</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1157,7 +1157,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>7157796.22</v>
+        <v>5161299.613333333</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -1166,16 +1166,16 @@
         <v>0</v>
       </c>
       <c r="M14">
-        <v>10255650.464</v>
+        <v>7260573.632</v>
       </c>
       <c r="N14">
-        <v>7157796.220000003</v>
+        <v>5161299.613333335</v>
       </c>
       <c r="O14">
-        <v>17413446.684</v>
+        <v>12421873.24533333</v>
       </c>
       <c r="P14">
-        <v>82686595.53333333</v>
+        <v>58726423.428</v>
       </c>
     </row>
     <row r="15">
@@ -1198,13 +1198,13 @@
         </is>
       </c>
       <c r="F15">
-        <v>1069717134.167333</v>
+        <v>714807951.6113334</v>
       </c>
       <c r="G15">
-        <v>536829367.7606667</v>
+        <v>331542799.218</v>
       </c>
       <c r="H15">
-        <v>33572577.79333334</v>
+        <v>13402474.83066667</v>
       </c>
       <c r="I15">
         <v>1828563</v>
@@ -1219,16 +1219,16 @@
         <v>796200.5699999999</v>
       </c>
       <c r="M15">
-        <v>498518988.0433334</v>
+        <v>369066476.9926667</v>
       </c>
       <c r="N15">
-        <v>34368778.36333331</v>
+        <v>14198675.40066666</v>
       </c>
       <c r="O15">
-        <v>532887766.4066666</v>
+        <v>383265152.3933333</v>
       </c>
       <c r="P15">
-        <v>1069717134.167333</v>
+        <v>714807951.6113334</v>
       </c>
     </row>
     <row r="16">
@@ -1256,37 +1256,37 @@
         </is>
       </c>
       <c r="F16">
-        <v>11841792393.31387</v>
+        <v>9272535042.686871</v>
       </c>
       <c r="G16">
-        <v>9666900875.041704</v>
+        <v>7560904510.96641</v>
       </c>
       <c r="H16">
-        <v>1848780453.572</v>
+        <v>1566695590.284616</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16">
-        <v>13135042.30813829</v>
+        <v>7347157.237976693</v>
       </c>
       <c r="K16">
-        <v>5305114</v>
+        <v>4495401.068</v>
       </c>
       <c r="L16">
-        <v>1234732.749016667</v>
+        <v>794285.5574099999</v>
       </c>
       <c r="M16">
-        <v>306579891.0430086</v>
+        <v>132441812.9724574</v>
       </c>
       <c r="N16">
-        <v>1868311627.229155</v>
+        <v>1579188718.748003</v>
       </c>
       <c r="O16">
-        <v>2174891518.272163</v>
+        <v>1711630531.72046</v>
       </c>
       <c r="P16">
-        <v>11841792393.31387</v>
+        <v>9272535042.686871</v>
       </c>
     </row>
     <row r="17">
@@ -1314,37 +1314,37 @@
         </is>
       </c>
       <c r="F17">
-        <v>7188624203.900336</v>
+        <v>4377410868.451186</v>
       </c>
       <c r="G17">
-        <v>5709795957.504503</v>
+        <v>3469022208.558336</v>
       </c>
       <c r="H17">
-        <v>1029518737.3436</v>
+        <v>619799935.0174309</v>
       </c>
       <c r="I17">
         <v>0</v>
       </c>
       <c r="J17">
-        <v>291522577.6349326</v>
+        <v>193504931.2675993</v>
       </c>
       <c r="K17">
-        <v>13673611.66733333</v>
+        <v>8046624.260533334</v>
       </c>
       <c r="L17">
-        <v>49236209.057715</v>
+        <v>29104290.69196234</v>
       </c>
       <c r="M17">
-        <v>94877110.692252</v>
+        <v>57932878.65532453</v>
       </c>
       <c r="N17">
-        <v>1383951135.703581</v>
+        <v>850455781.2375259</v>
       </c>
       <c r="O17">
-        <v>1478828246.395833</v>
+        <v>908388659.8928505</v>
       </c>
       <c r="P17">
-        <v>7188624203.900336</v>
+        <v>4377410868.451186</v>
       </c>
     </row>
     <row r="18">
@@ -1372,37 +1372,37 @@
         </is>
       </c>
       <c r="F18">
-        <v>3800712649.195081</v>
+        <v>2659996810.043734</v>
       </c>
       <c r="G18">
-        <v>3135264244.851837</v>
+        <v>2162226140.549317</v>
       </c>
       <c r="H18">
-        <v>511575015.6624787</v>
+        <v>388478186.8415329</v>
       </c>
       <c r="I18">
         <v>0</v>
       </c>
       <c r="J18">
-        <v>95972040.09472013</v>
+        <v>77797060.16551216</v>
       </c>
       <c r="K18">
-        <v>38163646.996</v>
+        <v>21046964.384</v>
       </c>
       <c r="L18">
-        <v>615806.9039333333</v>
+        <v>465531.83836</v>
       </c>
       <c r="M18">
-        <v>17532113.98277891</v>
+        <v>9250777.141678495</v>
       </c>
       <c r="N18">
-        <v>647916290.3604655</v>
+        <v>488519892.3527384</v>
       </c>
       <c r="O18">
-        <v>665448404.3432444</v>
+        <v>497770669.494417</v>
       </c>
       <c r="P18">
-        <v>3800712649.195081</v>
+        <v>2659996810.043734</v>
       </c>
     </row>
     <row r="19">
@@ -1425,37 +1425,37 @@
         </is>
       </c>
       <c r="F19">
-        <v>7803592628.761657</v>
+        <v>4476403874.599484</v>
       </c>
       <c r="G19">
-        <v>6500432538.183282</v>
+        <v>3712095761.906749</v>
       </c>
       <c r="H19">
-        <v>692944587.597494</v>
+        <v>436826133.759419</v>
       </c>
       <c r="I19">
         <v>0</v>
       </c>
       <c r="J19">
-        <v>106839580.6898456</v>
+        <v>75461949.11562128</v>
       </c>
       <c r="K19">
-        <v>353287262.7593333</v>
+        <v>164943802.0874667</v>
       </c>
       <c r="L19">
-        <v>51545257.49900167</v>
+        <v>36468924.11326767</v>
       </c>
       <c r="M19">
-        <v>99099709.8460338</v>
+        <v>50791525.283627</v>
       </c>
       <c r="N19">
-        <v>1204060380.732341</v>
+        <v>713516587.4091079</v>
       </c>
       <c r="O19">
-        <v>1303160090.578375</v>
+        <v>764308112.692735</v>
       </c>
       <c r="P19">
-        <v>7803592628.761657</v>
+        <v>4476403874.599484</v>
       </c>
     </row>
     <row r="20">
@@ -1483,37 +1483,37 @@
         </is>
       </c>
       <c r="F20">
-        <v>26275006986.68038</v>
+        <v>17408946564.19867</v>
       </c>
       <c r="G20">
-        <v>13679264315.72714</v>
+        <v>9009648515.148666</v>
       </c>
       <c r="H20">
-        <v>365778719.6175238</v>
+        <v>195029042.6746667</v>
       </c>
       <c r="I20">
-        <v>16779668.79</v>
+        <v>16318420.45666667</v>
       </c>
       <c r="J20">
-        <v>798552454.8246666</v>
+        <v>591455886.7086667</v>
       </c>
       <c r="K20">
-        <v>3078004099.553429</v>
+        <v>2229637965.115334</v>
       </c>
       <c r="L20">
-        <v>353678588.968</v>
+        <v>160671163.344</v>
       </c>
       <c r="M20">
-        <v>7960391031.232952</v>
+        <v>5192080117.914666</v>
       </c>
       <c r="N20">
-        <v>4635351639.720285</v>
+        <v>3207217931.135334</v>
       </c>
       <c r="O20">
-        <v>12595742670.95324</v>
+        <v>8399298049.05</v>
       </c>
       <c r="P20">
-        <v>26275006986.68038</v>
+        <v>17408946564.19867</v>
       </c>
     </row>
     <row r="21">
@@ -1541,37 +1541,37 @@
         </is>
       </c>
       <c r="F21">
-        <v>2685876766.184667</v>
+        <v>1382805266.883333</v>
       </c>
       <c r="G21">
-        <v>2245816945.928667</v>
+        <v>1158043510.200667</v>
       </c>
       <c r="H21">
-        <v>161335399.744</v>
+        <v>82793366.67733333</v>
       </c>
       <c r="I21">
         <v>0</v>
       </c>
       <c r="J21">
-        <v>101471907.7386667</v>
+        <v>50444607.92399999</v>
       </c>
       <c r="K21">
-        <v>143871033.8706667</v>
+        <v>74053728.67200001</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21">
-        <v>33381478.90266667</v>
+        <v>17470053.40933333</v>
       </c>
       <c r="N21">
-        <v>406678341.3533333</v>
+        <v>207291703.2733333</v>
       </c>
       <c r="O21">
-        <v>440059820.256</v>
+        <v>224761756.6826667</v>
       </c>
       <c r="P21">
-        <v>2685876766.184667</v>
+        <v>1382805266.883333</v>
       </c>
     </row>
     <row r="22">
@@ -1594,37 +1594,37 @@
         </is>
       </c>
       <c r="F22">
-        <v>35180318819.09463</v>
+        <v>26355633439.81809</v>
       </c>
       <c r="G22">
-        <v>23124889506.97476</v>
+        <v>17343558185.77667</v>
       </c>
       <c r="H22">
-        <v>417431096.6981633</v>
+        <v>309369834.216449</v>
       </c>
       <c r="I22">
-        <v>1932646264.902762</v>
+        <v>1460897681.306</v>
       </c>
       <c r="J22">
-        <v>1440554801.576571</v>
+        <v>903000617.9106667</v>
       </c>
       <c r="K22">
-        <v>391689089.6419261</v>
+        <v>309440772.3036743</v>
       </c>
       <c r="L22">
-        <v>41270444.59644677</v>
+        <v>34454805.61930392</v>
       </c>
       <c r="M22">
-        <v>557110633.686</v>
+        <v>387609932.1913334</v>
       </c>
       <c r="N22">
-        <v>11498318678.43387</v>
+        <v>8624465321.850094</v>
       </c>
       <c r="O22">
-        <v>12055429312.11987</v>
+        <v>9012075254.041428</v>
       </c>
       <c r="P22">
-        <v>35180318819.09463</v>
+        <v>26355633439.81809</v>
       </c>
     </row>
     <row r="23">
@@ -1652,37 +1652,37 @@
         </is>
       </c>
       <c r="F23">
-        <v>18203117966.40098</v>
+        <v>12098912043.82522</v>
       </c>
       <c r="G23">
-        <v>10237134772.06467</v>
+        <v>6895888196.87</v>
       </c>
       <c r="H23">
-        <v>928748297.2566667</v>
+        <v>630866815.7926667</v>
       </c>
       <c r="I23">
-        <v>2592094.266666667</v>
+        <v>1555256.56</v>
       </c>
       <c r="J23">
-        <v>196053079.1746667</v>
+        <v>141252199.984</v>
       </c>
       <c r="K23">
         <v>0</v>
       </c>
       <c r="L23">
-        <v>183966438.9053333</v>
+        <v>123057494.504</v>
       </c>
       <c r="M23">
-        <v>6669229310.830316</v>
+        <v>4316179972.87855</v>
       </c>
       <c r="N23">
-        <v>1296753883.506</v>
+        <v>886843874.0766668</v>
       </c>
       <c r="O23">
-        <v>7965983194.336316</v>
+        <v>5203023846.955216</v>
       </c>
       <c r="P23">
-        <v>18203117966.40098</v>
+        <v>12098912043.82522</v>
       </c>
     </row>
     <row r="24">
@@ -1710,37 +1710,37 @@
         </is>
       </c>
       <c r="F24">
-        <v>16425004.4635523</v>
+        <v>9549867.688682767</v>
       </c>
       <c r="G24">
-        <v>14924251.91764259</v>
+        <v>8677296.344283253</v>
       </c>
       <c r="H24">
-        <v>1081253.060326587</v>
+        <v>620463.3763903262</v>
       </c>
       <c r="I24">
         <v>0</v>
       </c>
       <c r="J24">
-        <v>226003.0904417069</v>
+        <v>145300.6346833072</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="L24">
-        <v>20824.06235</v>
+        <v>12494.43741</v>
       </c>
       <c r="M24">
-        <v>172672.3327914156</v>
+        <v>94312.89591587881</v>
       </c>
       <c r="N24">
-        <v>1328080.213118294</v>
+        <v>778258.4484836332</v>
       </c>
       <c r="O24">
-        <v>1500752.545909709</v>
+        <v>872571.344399512</v>
       </c>
       <c r="P24">
-        <v>16425004.4635523</v>
+        <v>9549867.688682767</v>
       </c>
     </row>
     <row r="25">
@@ -1768,37 +1768,37 @@
         </is>
       </c>
       <c r="F25">
-        <v>1929884073.117905</v>
+        <v>1215971703.026052</v>
       </c>
       <c r="G25">
-        <v>1775721070.197443</v>
+        <v>1118560954.959909</v>
       </c>
       <c r="H25">
-        <v>66487912.36421461</v>
+        <v>41543647.53844037</v>
       </c>
       <c r="I25">
         <v>0</v>
       </c>
       <c r="J25">
-        <v>617815.6389598745</v>
+        <v>321766.9305145005</v>
       </c>
       <c r="K25">
-        <v>50219232.02733333</v>
+        <v>28313535.978</v>
       </c>
       <c r="L25">
-        <v>2104786.663933333</v>
+        <v>1498004.395693333</v>
       </c>
       <c r="M25">
-        <v>31486710.72935442</v>
+        <v>23204502.14282817</v>
       </c>
       <c r="N25">
-        <v>122676292.1911078</v>
+        <v>74206245.92331485</v>
       </c>
       <c r="O25">
-        <v>154163002.9204622</v>
+        <v>97410748.06614304</v>
       </c>
       <c r="P25">
-        <v>1929884073.117905</v>
+        <v>1215971703.026052</v>
       </c>
     </row>
     <row r="26">
@@ -1821,37 +1821,37 @@
         </is>
       </c>
       <c r="F26">
-        <v>15779909238.11649</v>
+        <v>9220330658.694563</v>
       </c>
       <c r="G26">
-        <v>12721955795.48026</v>
+        <v>7375839095.150329</v>
       </c>
       <c r="H26">
-        <v>1642142095.153437</v>
+        <v>926257540.9677211</v>
       </c>
       <c r="I26">
-        <v>53699582.45</v>
+        <v>26139854.19</v>
       </c>
       <c r="J26">
-        <v>175730682.4636284</v>
+        <v>118265092.7220927</v>
       </c>
       <c r="K26">
-        <v>73084276.15531196</v>
+        <v>46691758.41832568</v>
       </c>
       <c r="L26">
-        <v>7889886.232079414</v>
+        <v>5365878.999259414</v>
       </c>
       <c r="M26">
-        <v>1105049081.361781</v>
+        <v>721518607.7388351</v>
       </c>
       <c r="N26">
-        <v>1952904361.274457</v>
+        <v>1122972955.805399</v>
       </c>
       <c r="O26">
-        <v>3057953442.636238</v>
+        <v>1844491563.544234</v>
       </c>
       <c r="P26">
-        <v>15779909238.11649</v>
+        <v>9220330658.694563</v>
       </c>
     </row>
     <row r="27">
@@ -1879,10 +1879,10 @@
         </is>
       </c>
       <c r="F27">
-        <v>188186549.6973333</v>
+        <v>341027803.804</v>
       </c>
       <c r="G27">
-        <v>79671456.26800001</v>
+        <v>139630873.2413333</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -1900,16 +1900,16 @@
         <v>0</v>
       </c>
       <c r="M27">
-        <v>108515093.4293333</v>
+        <v>201396930.5626667</v>
       </c>
       <c r="N27">
-        <v>-7.636845111846923e-09</v>
+        <v>-8.490557471911113e-09</v>
       </c>
       <c r="O27">
-        <v>108515093.4293333</v>
+        <v>201396930.5626667</v>
       </c>
       <c r="P27">
-        <v>188186549.6973333</v>
+        <v>341027803.804</v>
       </c>
     </row>
     <row r="28">
@@ -1937,10 +1937,10 @@
         </is>
       </c>
       <c r="F28">
-        <v>636876546.4373333</v>
+        <v>512047572.1615672</v>
       </c>
       <c r="G28">
-        <v>354054753.432</v>
+        <v>286784089.8013334</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -1958,16 +1958,16 @@
         <v>0</v>
       </c>
       <c r="M28">
-        <v>282821793.0053333</v>
+        <v>225263482.3602338</v>
       </c>
       <c r="N28">
-        <v>-7.605801026026407e-09</v>
+        <v>-8.50607951482137e-09</v>
       </c>
       <c r="O28">
-        <v>282821793.0053333</v>
+        <v>225263482.3602338</v>
       </c>
       <c r="P28">
-        <v>636876546.4373333</v>
+        <v>512047572.1615672</v>
       </c>
     </row>
     <row r="29">
@@ -1995,16 +1995,16 @@
         </is>
       </c>
       <c r="F29">
-        <v>4292975243.02</v>
+        <v>4915070379.397333</v>
       </c>
       <c r="G29">
-        <v>1613123938.753333</v>
+        <v>1875635131.894667</v>
       </c>
       <c r="H29">
         <v>0</v>
       </c>
       <c r="I29">
-        <v>546310</v>
+        <v>327786</v>
       </c>
       <c r="J29">
         <v>0</v>
@@ -2016,16 +2016,16 @@
         <v>0</v>
       </c>
       <c r="M29">
-        <v>2679304994.266666</v>
+        <v>3039107461.502666</v>
       </c>
       <c r="N29">
-        <v>546310.0000000171</v>
+        <v>327786.000000004</v>
       </c>
       <c r="O29">
-        <v>2679851304.266666</v>
+        <v>3039435247.502666</v>
       </c>
       <c r="P29">
-        <v>4292975243.02</v>
+        <v>4915070379.397333</v>
       </c>
     </row>
     <row r="30">
@@ -2048,10 +2048,10 @@
         </is>
       </c>
       <c r="F30">
-        <v>4531576187.509333</v>
+        <v>4062930487.330667</v>
       </c>
       <c r="G30">
-        <v>1836865517.26</v>
+        <v>1645618108.065333</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -2069,16 +2069,16 @@
         <v>0</v>
       </c>
       <c r="M30">
-        <v>2694710670.249333</v>
+        <v>2417312379.265333</v>
       </c>
       <c r="N30">
-        <v>4.38808153072993e-08</v>
+        <v>3.699290876587232e-08</v>
       </c>
       <c r="O30">
-        <v>2694710670.249333</v>
+        <v>2417312379.265333</v>
       </c>
       <c r="P30">
-        <v>4531576187.509333</v>
+        <v>4062930487.330667</v>
       </c>
     </row>
     <row r="31">
@@ -2102,20 +2102,20 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>EU2020_3</t>
+          <t>EU2020_2</t>
         </is>
       </c>
       <c r="F31">
-        <v>485547834.2066666</v>
+        <v>1839130.673333333</v>
       </c>
       <c r="G31">
-        <v>219707514.0666667</v>
+        <v>1379348.006666667</v>
       </c>
       <c r="H31">
         <v>0</v>
       </c>
       <c r="I31">
-        <v>0</v>
+        <v>817248.3333333333</v>
       </c>
       <c r="J31">
         <v>0</v>
@@ -2127,16 +2127,16 @@
         <v>0</v>
       </c>
       <c r="M31">
-        <v>265840320.14</v>
+        <v>459782.6666666666</v>
       </c>
       <c r="N31">
-        <v>-6.596868236859639e-10</v>
+        <v>-1.552204291025797e-10</v>
       </c>
       <c r="O31">
-        <v>265840320.14</v>
+        <v>459782.6666666665</v>
       </c>
       <c r="P31">
-        <v>485547834.2066666</v>
+        <v>1839130.673333333</v>
       </c>
     </row>
     <row r="32">
@@ -2158,11 +2158,16 @@
           <t>mssf</t>
         </is>
       </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>EU2020_3</t>
+        </is>
+      </c>
       <c r="F32">
-        <v>252732886.892</v>
+        <v>614334549.2973334</v>
       </c>
       <c r="G32">
-        <v>112290841.1426667</v>
+        <v>269428595.8346667</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -2180,16 +2185,16 @@
         <v>0</v>
       </c>
       <c r="M32">
-        <v>140442045.7493333</v>
+        <v>344905953.4626666</v>
       </c>
       <c r="N32">
-        <v>2.110997835795085e-09</v>
+        <v>-5.122274160385131e-10</v>
       </c>
       <c r="O32">
-        <v>140442045.7493333</v>
+        <v>344905953.4626666</v>
       </c>
       <c r="P32">
-        <v>252732886.892</v>
+        <v>614334549.2973334</v>
       </c>
     </row>
     <row r="33">
@@ -2203,7 +2208,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>AIS4</t>
+          <t>AIS3</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2211,16 +2216,11 @@
           <t>mssf</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>EU2020_2</t>
-        </is>
-      </c>
       <c r="F33">
-        <v>154178518.6933333</v>
+        <v>193283801.2293333</v>
       </c>
       <c r="G33">
-        <v>79568411.28666666</v>
+        <v>86139559.81333333</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -2238,16 +2238,16 @@
         <v>0</v>
       </c>
       <c r="M33">
-        <v>74610107.40666665</v>
+        <v>107144241.416</v>
       </c>
       <c r="N33">
-        <v>1.552204291025797e-10</v>
+        <v>1.785034934679667e-09</v>
       </c>
       <c r="O33">
-        <v>74610107.40666665</v>
+        <v>107144241.416</v>
       </c>
       <c r="P33">
-        <v>154178518.6933333</v>
+        <v>193283801.2293333</v>
       </c>
     </row>
     <row r="34">
@@ -2271,14 +2271,14 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>EU2020_3</t>
+          <t>EU2020_2</t>
         </is>
       </c>
       <c r="F34">
-        <v>1035502830.105333</v>
+        <v>149696186.032</v>
       </c>
       <c r="G34">
-        <v>390339051.7493333</v>
+        <v>77248871.57999998</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -2296,16 +2296,16 @@
         <v>0</v>
       </c>
       <c r="M34">
-        <v>645163778.3559999</v>
+        <v>72447314.45199999</v>
       </c>
       <c r="N34">
-        <v>5.712111790974934e-09</v>
+        <v>1.45907203356425e-09</v>
       </c>
       <c r="O34">
-        <v>645163778.3559999</v>
+        <v>72447314.45199999</v>
       </c>
       <c r="P34">
-        <v>1035502830.105333</v>
+        <v>149696186.032</v>
       </c>
     </row>
     <row r="35">
@@ -2327,11 +2327,16 @@
           <t>mssf</t>
         </is>
       </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>EU2020_3</t>
+        </is>
+      </c>
       <c r="F35">
-        <v>39512049.16</v>
+        <v>972365475.4106667</v>
       </c>
       <c r="G35">
-        <v>12425114.56</v>
+        <v>377199770.4933333</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -2349,16 +2354,16 @@
         <v>0</v>
       </c>
       <c r="M35">
-        <v>27086934.6</v>
+        <v>595165704.9173334</v>
       </c>
       <c r="N35">
-        <v>-4.811833302179973e-09</v>
+        <v>4.687656958897908e-09</v>
       </c>
       <c r="O35">
-        <v>27086934.59999999</v>
+        <v>595165704.9173334</v>
       </c>
       <c r="P35">
-        <v>39512049.16</v>
+        <v>972365475.4106667</v>
       </c>
     </row>
     <row r="36">
@@ -2372,7 +2377,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>AIS5</t>
+          <t>AIS4</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -2380,16 +2385,11 @@
           <t>mssf</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>EU2020_2</t>
-        </is>
-      </c>
       <c r="F36">
-        <v>269432579.5986667</v>
+        <v>78021589.41733333</v>
       </c>
       <c r="G36">
-        <v>142719982.3266667</v>
+        <v>30518146.09733333</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -2398,7 +2398,7 @@
         <v>0</v>
       </c>
       <c r="J36">
-        <v>57624824.37066667</v>
+        <v>0</v>
       </c>
       <c r="K36">
         <v>0</v>
@@ -2407,16 +2407,16 @@
         <v>0</v>
       </c>
       <c r="M36">
-        <v>69087772.90133333</v>
+        <v>47503443.32</v>
       </c>
       <c r="N36">
-        <v>57624824.37066667</v>
+        <v>-1.955777406692505e-09</v>
       </c>
       <c r="O36">
-        <v>126712597.272</v>
+        <v>47503443.31999999</v>
       </c>
       <c r="P36">
-        <v>269432579.5986667</v>
+        <v>78021589.41733333</v>
       </c>
     </row>
     <row r="37">
@@ -2440,14 +2440,14 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>EU2020_3</t>
+          <t>EU2020_2</t>
         </is>
       </c>
       <c r="F37">
-        <v>840589997.248</v>
+        <v>306474122.34</v>
       </c>
       <c r="G37">
-        <v>350599372.3733333</v>
+        <v>163216276.3773333</v>
       </c>
       <c r="H37">
         <v>0</v>
@@ -2456,25 +2456,25 @@
         <v>0</v>
       </c>
       <c r="J37">
-        <v>0</v>
+        <v>59132536.63733333</v>
       </c>
       <c r="K37">
         <v>0</v>
       </c>
       <c r="L37">
-        <v>2156200.006666666</v>
+        <v>0</v>
       </c>
       <c r="M37">
-        <v>487834424.868</v>
+        <v>84125309.32533333</v>
       </c>
       <c r="N37">
-        <v>2156200.006666669</v>
+        <v>59132536.63733333</v>
       </c>
       <c r="O37">
-        <v>489990624.8746667</v>
+        <v>143257845.9626667</v>
       </c>
       <c r="P37">
-        <v>840589997.248</v>
+        <v>306474122.34</v>
       </c>
     </row>
     <row r="38">
@@ -2498,14 +2498,14 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>EU2020_5</t>
+          <t>EU2020_3</t>
         </is>
       </c>
       <c r="F38">
-        <v>8016037.726666667</v>
+        <v>1094131757.352</v>
       </c>
       <c r="G38">
-        <v>6813632.058666667</v>
+        <v>462117425.9946666</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -2520,19 +2520,19 @@
         <v>0</v>
       </c>
       <c r="L38">
-        <v>0</v>
+        <v>14732866.67333333</v>
       </c>
       <c r="M38">
-        <v>1202405.668</v>
+        <v>629858131.3506666</v>
       </c>
       <c r="N38">
-        <v>0</v>
+        <v>2156200.006666669</v>
       </c>
       <c r="O38">
-        <v>1202405.668</v>
+        <v>632014331.3573333</v>
       </c>
       <c r="P38">
-        <v>8016037.726666667</v>
+        <v>1094131757.352</v>
       </c>
     </row>
     <row r="39">
@@ -2554,20 +2554,25 @@
           <t>mssf</t>
         </is>
       </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>EU2020_5</t>
+        </is>
+      </c>
       <c r="F39">
-        <v>1181947705.814667</v>
+        <v>26967382.416</v>
       </c>
       <c r="G39">
-        <v>527454075.2413333</v>
+        <v>21906849.02533333</v>
       </c>
       <c r="H39">
-        <v>16587116.74666667</v>
+        <v>0</v>
       </c>
       <c r="I39">
         <v>0</v>
       </c>
       <c r="J39">
-        <v>0</v>
+        <v>1450608.606666666</v>
       </c>
       <c r="K39">
         <v>0</v>
@@ -2576,16 +2581,16 @@
         <v>0</v>
       </c>
       <c r="M39">
-        <v>637906513.8266667</v>
+        <v>3609924.784</v>
       </c>
       <c r="N39">
-        <v>16587116.74666666</v>
+        <v>1450608.606666667</v>
       </c>
       <c r="O39">
-        <v>654493630.5733333</v>
+        <v>5060533.390666666</v>
       </c>
       <c r="P39">
-        <v>1181947705.814667</v>
+        <v>26967382.416</v>
       </c>
     </row>
     <row r="40">
@@ -2594,12 +2599,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>HC</t>
+          <t>AIS</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>HC</t>
+          <t>AIS5</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -2607,43 +2612,38 @@
           <t>mssf</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>EU2020_1</t>
-        </is>
-      </c>
       <c r="F40">
-        <v>8452173370.666627</v>
+        <v>1162635207.002667</v>
       </c>
       <c r="G40">
-        <v>6997301427.858878</v>
+        <v>549931375.776</v>
       </c>
       <c r="H40">
-        <v>1369245524.32261</v>
+        <v>26804949.66133333</v>
       </c>
       <c r="I40">
         <v>0</v>
       </c>
       <c r="J40">
-        <v>20448795.05627659</v>
+        <v>0</v>
       </c>
       <c r="K40">
-        <v>7561193.819999999</v>
+        <v>0</v>
       </c>
       <c r="L40">
-        <v>595373.5580333333</v>
+        <v>0</v>
       </c>
       <c r="M40">
-        <v>56957056.05082805</v>
+        <v>585898881.5653334</v>
       </c>
       <c r="N40">
-        <v>1397914886.75692</v>
+        <v>26804949.66133332</v>
       </c>
       <c r="O40">
-        <v>1454871942.807748</v>
+        <v>612703831.2266667</v>
       </c>
       <c r="P40">
-        <v>8452173370.666627</v>
+        <v>1162635207.002667</v>
       </c>
     </row>
     <row r="41">
@@ -2667,41 +2667,41 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>EU2020_4</t>
+          <t>EU2020_1</t>
         </is>
       </c>
       <c r="F41">
-        <v>6875205033.605473</v>
+        <v>9590610556.453983</v>
       </c>
       <c r="G41">
-        <v>5529755256.041739</v>
+        <v>7899702604.575979</v>
       </c>
       <c r="H41">
-        <v>950867164.6642681</v>
+        <v>1441828400.576349</v>
       </c>
       <c r="I41">
         <v>0</v>
       </c>
       <c r="J41">
-        <v>185904752.6298653</v>
+        <v>14544996.03595339</v>
       </c>
       <c r="K41">
-        <v>20455993.07966667</v>
+        <v>6572918.676</v>
       </c>
       <c r="L41">
-        <v>89402207.61543</v>
+        <v>1010831.87482</v>
       </c>
       <c r="M41">
-        <v>98819659.574504</v>
+        <v>226886804.7148823</v>
       </c>
       <c r="N41">
-        <v>1246630117.98923</v>
+        <v>1464021147.163122</v>
       </c>
       <c r="O41">
-        <v>1345449777.563734</v>
+        <v>1690907951.878004</v>
       </c>
       <c r="P41">
-        <v>6875205033.605473</v>
+        <v>9590610556.453983</v>
       </c>
     </row>
     <row r="42">
@@ -2725,41 +2725,41 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>EU2020_5</t>
+          <t>EU2020_4</t>
         </is>
       </c>
       <c r="F42">
-        <v>4120171336.18122</v>
+        <v>6548602260.052173</v>
       </c>
       <c r="G42">
-        <v>3282674033.555999</v>
+        <v>5230551950.404282</v>
       </c>
       <c r="H42">
-        <v>694387436.1408254</v>
+        <v>930390120.7210517</v>
       </c>
       <c r="I42">
         <v>0</v>
       </c>
       <c r="J42">
-        <v>123087108.3894403</v>
+        <v>234305794.6751987</v>
       </c>
       <c r="K42">
-        <v>14720097.852</v>
+        <v>15035828.29706667</v>
       </c>
       <c r="L42">
-        <v>739303.1878666666</v>
+        <v>56764095.84392467</v>
       </c>
       <c r="M42">
-        <v>3646690.388421399</v>
+        <v>81554470.11064908</v>
       </c>
       <c r="N42">
-        <v>833850612.236799</v>
+        <v>1236495839.537242</v>
       </c>
       <c r="O42">
-        <v>837497302.6252203</v>
+        <v>1318050309.647891</v>
       </c>
       <c r="P42">
-        <v>4120171336.18122</v>
+        <v>6548602260.052173</v>
       </c>
     </row>
     <row r="43">
@@ -2781,38 +2781,43 @@
           <t>mssf</t>
         </is>
       </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>EU2020_5</t>
+        </is>
+      </c>
       <c r="F43">
-        <v>5424352964.391877</v>
+        <v>4418702009.561075</v>
       </c>
       <c r="G43">
-        <v>4479764223.86314</v>
+        <v>3573592744.796557</v>
       </c>
       <c r="H43">
-        <v>597511043.0685962</v>
+        <v>681111021.5208379</v>
       </c>
       <c r="I43">
         <v>0</v>
       </c>
       <c r="J43">
-        <v>97580547.27969113</v>
+        <v>120330217.7710243</v>
       </c>
       <c r="K43">
-        <v>92843562.95366666</v>
+        <v>29541881.588</v>
       </c>
       <c r="L43">
-        <v>97723125.49800333</v>
+        <v>861385.67672</v>
       </c>
       <c r="M43">
-        <v>58921354.69544668</v>
+        <v>11800459.96126898</v>
       </c>
       <c r="N43">
-        <v>885667385.8332907</v>
+        <v>833308804.8032489</v>
       </c>
       <c r="O43">
-        <v>944588740.5287374</v>
+        <v>845109264.7645179</v>
       </c>
       <c r="P43">
-        <v>5424352964.391877</v>
+        <v>4418702009.561075</v>
       </c>
     </row>
     <row r="44">
@@ -2821,12 +2826,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>INFR</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>INFR</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -2834,43 +2839,38 @@
           <t>mssf</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>EU2020_3</t>
-        </is>
-      </c>
       <c r="F44">
-        <v>17332800180.66076</v>
+        <v>6745052608.402607</v>
       </c>
       <c r="G44">
-        <v>9442525449.174286</v>
+        <v>5620886436.720085</v>
       </c>
       <c r="H44">
-        <v>197192110.0150476</v>
+        <v>629278564.6608781</v>
       </c>
       <c r="I44">
-        <v>28213303.88</v>
+        <v>0</v>
       </c>
       <c r="J44">
-        <v>905607838.4693333</v>
+        <v>99928337.79124255</v>
       </c>
       <c r="K44">
-        <v>2072343542.246857</v>
+        <v>244506172.4189333</v>
       </c>
       <c r="L44">
-        <v>165226317.756</v>
+        <v>71687388.26653534</v>
       </c>
       <c r="M44">
-        <v>4477559900.885904</v>
+        <v>79134151.87826546</v>
       </c>
       <c r="N44">
-        <v>3412714830.600571</v>
+        <v>1045032019.804256</v>
       </c>
       <c r="O44">
-        <v>7890274731.486476</v>
+        <v>1124166171.682521</v>
       </c>
       <c r="P44">
-        <v>17332800180.66076</v>
+        <v>6745052608.402607</v>
       </c>
     </row>
     <row r="45">
@@ -2894,41 +2894,41 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>EU2020_5</t>
+          <t>EU2020_3</t>
         </is>
       </c>
       <c r="F45">
-        <v>973902862.6693333</v>
+        <v>22712547356.59733</v>
       </c>
       <c r="G45">
-        <v>816594119.6173333</v>
+        <v>12095941256.17733</v>
       </c>
       <c r="H45">
-        <v>57971055.728</v>
+        <v>341692960.0293334</v>
       </c>
       <c r="I45">
-        <v>0</v>
+        <v>27290807.21333333</v>
       </c>
       <c r="J45">
-        <v>45913153.51733333</v>
+        <v>1010095541.557333</v>
       </c>
       <c r="K45">
-        <v>41773918.80133333</v>
+        <v>2503225750.710667</v>
       </c>
       <c r="L45">
-        <v>0</v>
+        <v>301143045.008</v>
       </c>
       <c r="M45">
-        <v>11650615.00533333</v>
+        <v>6409750757.529333</v>
       </c>
       <c r="N45">
-        <v>145658128.0466667</v>
+        <v>4206855342.890666</v>
       </c>
       <c r="O45">
-        <v>157308743.052</v>
+        <v>10616606100.42</v>
       </c>
       <c r="P45">
-        <v>973902862.6693333</v>
+        <v>22712547356.59733</v>
       </c>
     </row>
     <row r="46">
@@ -2950,38 +2950,43 @@
           <t>mssf</t>
         </is>
       </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>EU2020_5</t>
+        </is>
+      </c>
       <c r="F46">
-        <v>36991677247.19105</v>
+        <v>1971792342.986667</v>
       </c>
       <c r="G46">
-        <v>27846002406.24952</v>
+        <v>1645952713.201333</v>
       </c>
       <c r="H46">
-        <v>344313134.9967619</v>
+        <v>117988019.7346667</v>
       </c>
       <c r="I46">
-        <v>2537790205.665524</v>
+        <v>0</v>
       </c>
       <c r="J46">
-        <v>1329363726.933143</v>
+        <v>89336179.728</v>
       </c>
       <c r="K46">
-        <v>477748901.8811429</v>
+        <v>94623317.244</v>
       </c>
       <c r="L46">
-        <v>59015287.19695238</v>
+        <v>0</v>
       </c>
       <c r="M46">
-        <v>574292041.192</v>
+        <v>23892113.07866666</v>
       </c>
       <c r="N46">
-        <v>8571382799.749523</v>
+        <v>301947516.7066666</v>
       </c>
       <c r="O46">
-        <v>9145674840.941523</v>
+        <v>325839629.7853333</v>
       </c>
       <c r="P46">
-        <v>36991677247.19105</v>
+        <v>1971792342.986667</v>
       </c>
     </row>
     <row r="47">
@@ -2990,12 +2995,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>RD</t>
+          <t>INFR</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>RD</t>
+          <t>INFR</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3003,43 +3008,38 @@
           <t>mssf</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>EU2020_2</t>
-        </is>
-      </c>
       <c r="F47">
-        <v>20836113154.17467</v>
+        <v>35284603266.91901</v>
       </c>
       <c r="G47">
-        <v>12870271837.34133</v>
+        <v>25534443889.99333</v>
       </c>
       <c r="H47">
-        <v>1631442485.393333</v>
+        <v>396695140.5133333</v>
       </c>
       <c r="I47">
-        <v>5184188.533333333</v>
+        <v>2127605577.492</v>
       </c>
       <c r="J47">
-        <v>81884641.92933333</v>
+        <v>1519516822.581333</v>
       </c>
       <c r="K47">
-        <v>0</v>
+        <v>482209577.5656804</v>
       </c>
       <c r="L47">
-        <v>364027052.1106666</v>
+        <v>62339359.38266667</v>
       </c>
       <c r="M47">
-        <v>5912515001.061334</v>
+        <v>502087952.3226666</v>
       </c>
       <c r="N47">
-        <v>2053326315.772</v>
+        <v>9248071424.603014</v>
       </c>
       <c r="O47">
-        <v>7965841316.833333</v>
+        <v>9750159376.92568</v>
       </c>
       <c r="P47">
-        <v>20836113154.17467</v>
+        <v>35284603266.91901</v>
       </c>
     </row>
     <row r="48">
@@ -3048,12 +3048,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>TA</t>
+          <t>RD</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>TA</t>
+          <t>RD</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -3063,41 +3063,41 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>EU2020_1</t>
+          <t>EU2020_2</t>
         </is>
       </c>
       <c r="F48">
-        <v>23480875.70301327</v>
+        <v>17878025827.43443</v>
       </c>
       <c r="G48">
-        <v>21335428.16401502</v>
+        <v>10463501335.532</v>
       </c>
       <c r="H48">
-        <v>1433601.586442895</v>
+        <v>1127308892.325333</v>
       </c>
       <c r="I48">
-        <v>0</v>
+        <v>3110513.12</v>
       </c>
       <c r="J48">
-        <v>452006.1808834139</v>
+        <v>118887694.168</v>
       </c>
       <c r="K48">
         <v>0</v>
       </c>
       <c r="L48">
-        <v>41648.12470000001</v>
+        <v>242950241.928</v>
       </c>
       <c r="M48">
-        <v>218191.6469719418</v>
+        <v>5942042935.889099</v>
       </c>
       <c r="N48">
-        <v>1927255.892026309</v>
+        <v>1472481556.013333</v>
       </c>
       <c r="O48">
-        <v>2145447.538998251</v>
+        <v>7414524491.902433</v>
       </c>
       <c r="P48">
-        <v>23480875.70301327</v>
+        <v>17878025827.43443</v>
       </c>
     </row>
     <row r="49">
@@ -3121,41 +3121,41 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>EU2020_5</t>
+          <t>EU2020_1</t>
         </is>
       </c>
       <c r="F49">
-        <v>1306792200.365553</v>
+        <v>18321001.34572318</v>
       </c>
       <c r="G49">
-        <v>1183671983.74576</v>
+        <v>16647011.53300769</v>
       </c>
       <c r="H49">
-        <v>70398237.11496121</v>
+        <v>1192763.572864562</v>
       </c>
       <c r="I49">
         <v>0</v>
       </c>
       <c r="J49">
-        <v>555396.2779197489</v>
+        <v>290601.2693666145</v>
       </c>
       <c r="K49">
-        <v>14902693.17466667</v>
+        <v>0</v>
       </c>
       <c r="L49">
-        <v>2518582.867866667</v>
+        <v>24988.87482000001</v>
       </c>
       <c r="M49">
-        <v>32556559.67104527</v>
+        <v>165636.0956643135</v>
       </c>
       <c r="N49">
-        <v>90563656.94874761</v>
+        <v>1508353.717051177</v>
       </c>
       <c r="O49">
-        <v>123120216.6197929</v>
+        <v>1673989.81271549</v>
       </c>
       <c r="P49">
-        <v>1306792200.365553</v>
+        <v>18321001.34572318</v>
       </c>
     </row>
     <row r="50">
@@ -3177,52 +3177,57 @@
           <t>mssf</t>
         </is>
       </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>EU2020_5</t>
+        </is>
+      </c>
       <c r="F50">
-        <v>11521060545.24224</v>
+        <v>1683584576.384098</v>
       </c>
       <c r="G50">
-        <v>8768962744.623802</v>
+        <v>1545591317.851496</v>
       </c>
       <c r="H50">
-        <v>1177804450.968962</v>
+        <v>64555409.33030874</v>
       </c>
       <c r="I50">
-        <v>37447374.82</v>
+        <v>0</v>
       </c>
       <c r="J50">
-        <v>124897595.9472569</v>
+        <v>551033.861029001</v>
       </c>
       <c r="K50">
-        <v>44586904.19333334</v>
+        <v>31557065.456</v>
       </c>
       <c r="L50">
-        <v>4840443.9401</v>
+        <v>2375714.351386667</v>
       </c>
       <c r="M50">
-        <v>1362433499.088783</v>
+        <v>37182082.11254435</v>
       </c>
       <c r="N50">
-        <v>1389664301.529652</v>
+        <v>100811176.4200577</v>
       </c>
       <c r="O50">
-        <v>2752097800.618435</v>
+        <v>137993258.5326021</v>
       </c>
       <c r="P50">
-        <v>11521060545.24224</v>
+        <v>1683584576.384098</v>
       </c>
     </row>
     <row r="51">
       <c r="A51">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>AIS</t>
+          <t>TA</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>AIS1</t>
+          <t>TA</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -3230,43 +3235,38 @@
           <t>mssf</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>EU2020_3</t>
-        </is>
-      </c>
       <c r="F51">
-        <v>24262825.484</v>
+        <v>14634302367.63866</v>
       </c>
       <c r="G51">
-        <v>11059547.288</v>
+        <v>11665229867.58926</v>
       </c>
       <c r="H51">
-        <v>0</v>
+        <v>1631314730.748377</v>
       </c>
       <c r="I51">
-        <v>0</v>
+        <v>51640960.32</v>
       </c>
       <c r="J51">
-        <v>0</v>
+        <v>175063502.6641855</v>
       </c>
       <c r="K51">
-        <v>0</v>
+        <v>64692966.3583196</v>
       </c>
       <c r="L51">
-        <v>0</v>
+        <v>6596520.43446</v>
       </c>
       <c r="M51">
-        <v>13203278.196</v>
+        <v>1039579021.008059</v>
       </c>
       <c r="N51">
-        <v>-1.862645149230957e-10</v>
+        <v>1929493479.041342</v>
       </c>
       <c r="O51">
-        <v>13203278.196</v>
+        <v>2969072500.049401</v>
       </c>
       <c r="P51">
-        <v>24262825.484</v>
+        <v>14634302367.63866</v>
       </c>
     </row>
     <row r="52">
@@ -3280,7 +3280,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>AIS2</t>
+          <t>AIS1</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -3290,14 +3290,14 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>EU2020_2</t>
+          <t>EU2020_3</t>
         </is>
       </c>
       <c r="F52">
-        <v>72983948.704</v>
+        <v>101800023.584</v>
       </c>
       <c r="G52">
-        <v>39429118.832</v>
+        <v>43203670.168</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -3315,16 +3315,16 @@
         <v>0</v>
       </c>
       <c r="M52">
-        <v>33554829.872</v>
+        <v>58596353.416</v>
       </c>
       <c r="N52">
-        <v>0</v>
+        <v>-1.862645149230957e-10</v>
       </c>
       <c r="O52">
-        <v>33554829.872</v>
+        <v>58596353.416</v>
       </c>
       <c r="P52">
-        <v>72983948.704</v>
+        <v>101800023.584</v>
       </c>
     </row>
     <row r="53">
@@ -3348,14 +3348,14 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>EU2020_3</t>
+          <t>EU2020_2</t>
         </is>
       </c>
       <c r="F53">
-        <v>1201773949.76</v>
+        <v>396262061.052</v>
       </c>
       <c r="G53">
-        <v>430172710.74</v>
+        <v>218165283.508</v>
       </c>
       <c r="H53">
         <v>0</v>
@@ -3373,16 +3373,16 @@
         <v>0</v>
       </c>
       <c r="M53">
-        <v>771601239.02</v>
+        <v>178096777.544</v>
       </c>
       <c r="N53">
-        <v>8.568167686462403e-09</v>
+        <v>-5.867332220077515e-09</v>
       </c>
       <c r="O53">
-        <v>771601239.02</v>
+        <v>178096777.544</v>
       </c>
       <c r="P53">
-        <v>1201773949.76</v>
+        <v>396262061.052</v>
       </c>
     </row>
     <row r="54">
@@ -3404,17 +3404,22 @@
           <t>mssf</t>
         </is>
       </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>EU2020_3</t>
+        </is>
+      </c>
       <c r="F54">
-        <v>290660083.216</v>
+        <v>2397283635.404</v>
       </c>
       <c r="G54">
-        <v>115525955.04</v>
+        <v>879645250.928</v>
       </c>
       <c r="H54">
         <v>0</v>
       </c>
       <c r="I54">
-        <v>0</v>
+        <v>327786</v>
       </c>
       <c r="J54">
         <v>0</v>
@@ -3426,16 +3431,16 @@
         <v>0</v>
       </c>
       <c r="M54">
-        <v>175134128.176</v>
+        <v>1517310598.476</v>
       </c>
       <c r="N54">
-        <v>1.117587089538574e-09</v>
+        <v>327786.0000000151</v>
       </c>
       <c r="O54">
-        <v>175134128.176</v>
+        <v>1517638384.476</v>
       </c>
       <c r="P54">
-        <v>290660083.216</v>
+        <v>2397283635.404</v>
       </c>
     </row>
     <row r="55">
@@ -3449,7 +3454,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>AIS3</t>
+          <t>AIS2</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -3457,16 +3462,11 @@
           <t>mssf</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>EU2020_3</t>
-        </is>
-      </c>
       <c r="F55">
-        <v>30693989.6</v>
+        <v>2615911855.964</v>
       </c>
       <c r="G55">
-        <v>14209584.68</v>
+        <v>1057463714.192</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -3484,16 +3484,16 @@
         <v>0</v>
       </c>
       <c r="M55">
-        <v>16484404.92</v>
+        <v>1558448141.772</v>
       </c>
       <c r="N55">
-        <v>0</v>
+        <v>2.218876034021378e-08</v>
       </c>
       <c r="O55">
-        <v>16484404.92</v>
+        <v>1558448141.772</v>
       </c>
       <c r="P55">
-        <v>30693989.6</v>
+        <v>2615911855.964</v>
       </c>
     </row>
     <row r="56">
@@ -3515,11 +3515,16 @@
           <t>mssf</t>
         </is>
       </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>EU2020_3</t>
+        </is>
+      </c>
       <c r="F56">
-        <v>13127222.752</v>
+        <v>122477452.444</v>
       </c>
       <c r="G56">
-        <v>5907250.236</v>
+        <v>58469118.148</v>
       </c>
       <c r="H56">
         <v>0</v>
@@ -3537,16 +3542,16 @@
         <v>0</v>
       </c>
       <c r="M56">
-        <v>7219972.516</v>
+        <v>64008334.296</v>
       </c>
       <c r="N56">
-        <v>1.490116119384766e-09</v>
+        <v>6.98491930961609e-11</v>
       </c>
       <c r="O56">
-        <v>7219972.516000001</v>
+        <v>64008334.296</v>
       </c>
       <c r="P56">
-        <v>13127222.752</v>
+        <v>122477452.444</v>
       </c>
     </row>
     <row r="57">
@@ -3560,7 +3565,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>AIS4</t>
+          <t>AIS3</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -3568,16 +3573,11 @@
           <t>mssf</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>EU2020_3</t>
-        </is>
-      </c>
       <c r="F57">
-        <v>215257728.552</v>
+        <v>155821194.436</v>
       </c>
       <c r="G57">
-        <v>91368016.536</v>
+        <v>69256162.72</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -3595,16 +3595,16 @@
         <v>0</v>
       </c>
       <c r="M57">
-        <v>123889712.016</v>
+        <v>86565031.71600001</v>
       </c>
       <c r="N57">
-        <v>7.450580596923829e-10</v>
+        <v>1.862645149230957e-09</v>
       </c>
       <c r="O57">
-        <v>123889712.016</v>
+        <v>86565031.71600001</v>
       </c>
       <c r="P57">
-        <v>215257728.552</v>
+        <v>155821194.436</v>
       </c>
     </row>
     <row r="58">
@@ -3618,7 +3618,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>AIS5</t>
+          <t>AIS4</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -3632,10 +3632,10 @@
         </is>
       </c>
       <c r="F58">
-        <v>24264609.812</v>
+        <v>19305847.292</v>
       </c>
       <c r="G58">
-        <v>12314049.34</v>
+        <v>10214098.82</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -3644,7 +3644,7 @@
         <v>0</v>
       </c>
       <c r="J58">
-        <v>5006631.604</v>
+        <v>0</v>
       </c>
       <c r="K58">
         <v>0</v>
@@ -3653,16 +3653,16 @@
         <v>0</v>
       </c>
       <c r="M58">
-        <v>6943928.868</v>
+        <v>9091748.472000001</v>
       </c>
       <c r="N58">
-        <v>5006631.604000001</v>
+        <v>-9.313225746154786e-11</v>
       </c>
       <c r="O58">
-        <v>11950560.472</v>
+        <v>9091748.472000001</v>
       </c>
       <c r="P58">
-        <v>24264609.812</v>
+        <v>19305847.292</v>
       </c>
     </row>
     <row r="59">
@@ -3676,7 +3676,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>AIS5</t>
+          <t>AIS4</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -3690,10 +3690,10 @@
         </is>
       </c>
       <c r="F59">
-        <v>277772228.548</v>
+        <v>663013454.6440001</v>
       </c>
       <c r="G59">
-        <v>114674205.76</v>
+        <v>251437228.74</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -3711,16 +3711,16 @@
         <v>0</v>
       </c>
       <c r="M59">
-        <v>163098022.788</v>
+        <v>411576225.904</v>
       </c>
       <c r="N59">
-        <v>1.862645149230957e-10</v>
+        <v>3.67872416973114e-09</v>
       </c>
       <c r="O59">
-        <v>163098022.788</v>
+        <v>411576225.904</v>
       </c>
       <c r="P59">
-        <v>277772228.548</v>
+        <v>663013454.6440001</v>
       </c>
     </row>
     <row r="60">
@@ -3734,7 +3734,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>AIS5</t>
+          <t>AIS4</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -3742,16 +3742,11 @@
           <t>mssf</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>EU2020_5</t>
-        </is>
-      </c>
       <c r="F60">
-        <v>1487618.7</v>
+        <v>10602227.584</v>
       </c>
       <c r="G60">
-        <v>1264475.892</v>
+        <v>5025062.044</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -3769,16 +3764,16 @@
         <v>0</v>
       </c>
       <c r="M60">
-        <v>223142.808</v>
+        <v>5577165.54</v>
       </c>
       <c r="N60">
-        <v>0</v>
+        <v>-1.024454832077026e-09</v>
       </c>
       <c r="O60">
-        <v>223142.808</v>
+        <v>5577165.54</v>
       </c>
       <c r="P60">
-        <v>1487618.7</v>
+        <v>10602227.584</v>
       </c>
     </row>
     <row r="61">
@@ -3800,11 +3795,16 @@
           <t>mssf</t>
         </is>
       </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>EU2020_2</t>
+        </is>
+      </c>
       <c r="F61">
-        <v>439017798.928</v>
+        <v>64362832.66</v>
       </c>
       <c r="G61">
-        <v>191312981.808</v>
+        <v>33977526.064</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -3813,7 +3813,7 @@
         <v>0</v>
       </c>
       <c r="J61">
-        <v>0</v>
+        <v>5006631.604</v>
       </c>
       <c r="K61">
         <v>0</v>
@@ -3822,16 +3822,16 @@
         <v>0</v>
       </c>
       <c r="M61">
-        <v>247704817.12</v>
+        <v>25378674.992</v>
       </c>
       <c r="N61">
-        <v>7.450580596923828e-09</v>
+        <v>5006631.604000001</v>
       </c>
       <c r="O61">
-        <v>247704817.12</v>
+        <v>30385306.596</v>
       </c>
       <c r="P61">
-        <v>439017798.928</v>
+        <v>64362832.66</v>
       </c>
     </row>
     <row r="62">
@@ -3840,12 +3840,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>HC</t>
+          <t>AIS</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>HC</t>
+          <t>AIS5</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -3855,23 +3855,23 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>EU2020_1</t>
+          <t>EU2020_3</t>
         </is>
       </c>
       <c r="F62">
-        <v>1945181243.798025</v>
+        <v>482149984.552</v>
       </c>
       <c r="G62">
-        <v>1577903181.307394</v>
+        <v>203744931.088</v>
       </c>
       <c r="H62">
-        <v>366143782.1451625</v>
+        <v>0</v>
       </c>
       <c r="I62">
         <v>0</v>
       </c>
       <c r="J62">
-        <v>692126.9054685847</v>
+        <v>0</v>
       </c>
       <c r="K62">
         <v>0</v>
@@ -3880,16 +3880,16 @@
         <v>0</v>
       </c>
       <c r="M62">
-        <v>442153.44</v>
+        <v>278405053.464</v>
       </c>
       <c r="N62">
-        <v>366835909.0506311</v>
+        <v>-4.190951585769653e-10</v>
       </c>
       <c r="O62">
-        <v>367278062.4906311</v>
+        <v>278405053.464</v>
       </c>
       <c r="P62">
-        <v>1945181243.798025</v>
+        <v>482149984.552</v>
       </c>
     </row>
     <row r="63">
@@ -3898,12 +3898,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>HC</t>
+          <t>AIS</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>HC</t>
+          <t>AIS5</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -3913,23 +3913,23 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>EU2020_4</t>
+          <t>EU2020_5</t>
         </is>
       </c>
       <c r="F63">
-        <v>474141668.615388</v>
+        <v>6496446.116</v>
       </c>
       <c r="G63">
-        <v>396092620.2017372</v>
+        <v>5139857.592</v>
       </c>
       <c r="H63">
-        <v>65382204.95911881</v>
+        <v>0</v>
       </c>
       <c r="I63">
         <v>0</v>
       </c>
       <c r="J63">
-        <v>12641625.966532</v>
+        <v>545888</v>
       </c>
       <c r="K63">
         <v>0</v>
@@ -3938,16 +3938,16 @@
         <v>0</v>
       </c>
       <c r="M63">
-        <v>25217.488</v>
+        <v>810700.524</v>
       </c>
       <c r="N63">
-        <v>78023830.92565081</v>
+        <v>545888</v>
       </c>
       <c r="O63">
-        <v>78049048.41365081</v>
+        <v>1356588.524</v>
       </c>
       <c r="P63">
-        <v>474141668.615388</v>
+        <v>6496446.116</v>
       </c>
     </row>
     <row r="64">
@@ -3956,12 +3956,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>HC</t>
+          <t>AIS</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>HC</t>
+          <t>AIS5</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -3969,43 +3969,38 @@
           <t>mssf</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>EU2020_5</t>
-        </is>
-      </c>
       <c r="F64">
-        <v>159780343.4104896</v>
+        <v>813239480.296</v>
       </c>
       <c r="G64">
-        <v>94808535.95654695</v>
+        <v>374122249.816</v>
       </c>
       <c r="H64">
-        <v>47132730.25720892</v>
+        <v>9952270.048</v>
       </c>
       <c r="I64">
         <v>0</v>
       </c>
       <c r="J64">
-        <v>17269474.21673379</v>
+        <v>0</v>
       </c>
       <c r="K64">
-        <v>464265.552</v>
+        <v>0</v>
       </c>
       <c r="L64">
         <v>0</v>
       </c>
       <c r="M64">
-        <v>105337.428</v>
+        <v>429164960.432</v>
       </c>
       <c r="N64">
-        <v>64866470.02594271</v>
+        <v>9952270.048</v>
       </c>
       <c r="O64">
-        <v>64971807.45394271</v>
+        <v>439117230.48</v>
       </c>
       <c r="P64">
-        <v>159780343.4104896</v>
+        <v>813239480.296</v>
       </c>
     </row>
     <row r="65">
@@ -4027,38 +4022,43 @@
           <t>mssf</t>
         </is>
       </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>EU2020_1</t>
+        </is>
+      </c>
       <c r="F65">
-        <v>1319825781.505392</v>
+        <v>3376001408.637666</v>
       </c>
       <c r="G65">
-        <v>1097798797.801383</v>
+        <v>2781498368.665587</v>
       </c>
       <c r="H65">
-        <v>153147427.3114392</v>
+        <v>575645769.1788079</v>
       </c>
       <c r="I65">
         <v>0</v>
       </c>
       <c r="J65">
-        <v>36968226.7885697</v>
+        <v>12383810.99595339</v>
       </c>
       <c r="K65">
-        <v>5397630.34</v>
+        <v>1797988.076</v>
       </c>
       <c r="L65">
-        <v>26401586.776</v>
+        <v>24988.87482000001</v>
       </c>
       <c r="M65">
-        <v>112112.488</v>
+        <v>4650482.846496835</v>
       </c>
       <c r="N65">
-        <v>221914871.2160089</v>
+        <v>589852557.1255814</v>
       </c>
       <c r="O65">
-        <v>222026983.7040089</v>
+        <v>594503039.9720782</v>
       </c>
       <c r="P65">
-        <v>1319825781.505392</v>
+        <v>3376001408.637666</v>
       </c>
     </row>
     <row r="66">
@@ -4067,12 +4067,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>INFR</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>INFR</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -4082,41 +4082,41 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>EU2020_3</t>
+          <t>EU2020_4</t>
         </is>
       </c>
       <c r="F66">
-        <v>8031644810.427429</v>
+        <v>3611957777.617839</v>
       </c>
       <c r="G66">
-        <v>4444154832.554286</v>
+        <v>2936069674.785362</v>
       </c>
       <c r="H66">
-        <v>96970531.52171429</v>
+        <v>495578051.2285044</v>
       </c>
       <c r="I66">
-        <v>12881678.16</v>
+        <v>0</v>
       </c>
       <c r="J66">
-        <v>474471975.076</v>
+        <v>62258230.288532</v>
       </c>
       <c r="K66">
-        <v>790364002.9468572</v>
+        <v>11047152.1894</v>
       </c>
       <c r="L66">
-        <v>54227922.736</v>
+        <v>52770030.137258</v>
       </c>
       <c r="M66">
-        <v>2152298163.432571</v>
+        <v>54234638.98878241</v>
       </c>
       <c r="N66">
-        <v>1435191814.440572</v>
+        <v>621653463.8436944</v>
       </c>
       <c r="O66">
-        <v>3587489977.873143</v>
+        <v>675888102.8324769</v>
       </c>
       <c r="P66">
-        <v>8031644810.427429</v>
+        <v>3611957777.617839</v>
       </c>
     </row>
     <row r="67">
@@ -4125,12 +4125,12 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>INFR</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>INFR</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -4144,37 +4144,37 @@
         </is>
       </c>
       <c r="F67">
-        <v>278476410.516</v>
+        <v>1001965509.181981</v>
       </c>
       <c r="G67">
-        <v>236788828.904</v>
+        <v>776927929.0185087</v>
       </c>
       <c r="H67">
-        <v>18337241.288</v>
+        <v>183505973.6981422</v>
       </c>
       <c r="I67">
         <v>0</v>
       </c>
       <c r="J67">
-        <v>11283794.504</v>
+        <v>38201344.76435766</v>
       </c>
       <c r="K67">
-        <v>7611185.048</v>
+        <v>2759164.428</v>
       </c>
       <c r="L67">
-        <v>0</v>
+        <v>28192.57672000001</v>
       </c>
       <c r="M67">
-        <v>4455360.772</v>
+        <v>232904.6962528394</v>
       </c>
       <c r="N67">
-        <v>37232220.84</v>
+        <v>224804675.4672199</v>
       </c>
       <c r="O67">
-        <v>41687581.612</v>
+        <v>225037580.1634727</v>
       </c>
       <c r="P67">
-        <v>278476410.516</v>
+        <v>1001965509.181981</v>
       </c>
     </row>
     <row r="68">
@@ -4183,12 +4183,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>INFR</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>INFR</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -4197,37 +4197,37 @@
         </is>
       </c>
       <c r="F68">
-        <v>12944729691.95771</v>
+        <v>3326314891.656836</v>
       </c>
       <c r="G68">
-        <v>10142355769.28286</v>
+        <v>2745013361.220971</v>
       </c>
       <c r="H68">
-        <v>156025225.3634286</v>
+        <v>377498359.5572324</v>
       </c>
       <c r="I68">
-        <v>825719261.5188572</v>
+        <v>0</v>
       </c>
       <c r="J68">
-        <v>491434978.7131429</v>
+        <v>65998067.85124256</v>
       </c>
       <c r="K68">
-        <v>213616994.3811429</v>
+        <v>42078481.5466</v>
       </c>
       <c r="L68">
-        <v>29913239.05028572</v>
+        <v>67513657.39320201</v>
       </c>
       <c r="M68">
-        <v>102903712.832</v>
+        <v>28207499.86758802</v>
       </c>
       <c r="N68">
-        <v>2699470209.842857</v>
+        <v>553094030.568277</v>
       </c>
       <c r="O68">
-        <v>2802373922.674857</v>
+        <v>581301530.435865</v>
       </c>
       <c r="P68">
-        <v>12944729691.95771</v>
+        <v>3326314891.656836</v>
       </c>
     </row>
     <row r="69">
@@ -4236,12 +4236,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>RD</t>
+          <t>INFR</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>RD</t>
+          <t>INFR</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -4251,41 +4251,41 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>EU2020_2</t>
+          <t>EU2020_3</t>
         </is>
       </c>
       <c r="F69">
-        <v>3945197763.228</v>
+        <v>11808226473.684</v>
       </c>
       <c r="G69">
-        <v>2243230362.428</v>
+        <v>6575193663.864</v>
       </c>
       <c r="H69">
-        <v>229411936.12</v>
+        <v>123274672.736</v>
       </c>
       <c r="I69">
-        <v>0</v>
+        <v>14265423.16</v>
       </c>
       <c r="J69">
-        <v>32979318.656</v>
+        <v>592123544.404</v>
       </c>
       <c r="K69">
-        <v>0</v>
+        <v>1334429880.064</v>
       </c>
       <c r="L69">
-        <v>48143445.724</v>
+        <v>111318621.108</v>
       </c>
       <c r="M69">
-        <v>1397054085.828</v>
+        <v>3022167829.356</v>
       </c>
       <c r="N69">
-        <v>304913314.9719999</v>
+        <v>2210864980.464</v>
       </c>
       <c r="O69">
-        <v>1701967400.8</v>
+        <v>5233032809.82</v>
       </c>
       <c r="P69">
-        <v>3945197763.228</v>
+        <v>11808226473.684</v>
       </c>
     </row>
     <row r="70">
@@ -4294,12 +4294,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>TA</t>
+          <t>INFR</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>TA</t>
+          <t>INFR</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -4309,41 +4309,41 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>EU2020_1</t>
+          <t>EU2020_5</t>
         </is>
       </c>
       <c r="F70">
-        <v>3279311.890415085</v>
+        <v>583658429.5</v>
       </c>
       <c r="G70">
-        <v>2979681.167166119</v>
+        <v>495203671.048</v>
       </c>
       <c r="H70">
-        <v>251136.8211575505</v>
+        <v>36862310.348</v>
       </c>
       <c r="I70">
         <v>0</v>
       </c>
       <c r="J70">
-        <v>48493.9020914153</v>
+        <v>18888068.108</v>
       </c>
       <c r="K70">
-        <v>0</v>
+        <v>24579091.804</v>
       </c>
       <c r="L70">
         <v>0</v>
       </c>
       <c r="M70">
-        <v>0</v>
+        <v>8125288.192000001</v>
       </c>
       <c r="N70">
-        <v>299630.723248966</v>
+        <v>80329470.26000001</v>
       </c>
       <c r="O70">
-        <v>299630.723248966</v>
+        <v>88454758.45200001</v>
       </c>
       <c r="P70">
-        <v>3279311.890415085</v>
+        <v>583658429.5</v>
       </c>
     </row>
     <row r="71">
@@ -4352,12 +4352,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>TA</t>
+          <t>INFR</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>TA</t>
+          <t>INFR</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -4365,43 +4365,38 @@
           <t>mssf</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>EU2020_5</t>
-        </is>
-      </c>
       <c r="F71">
-        <v>493263825.3277504</v>
+        <v>24460796928.492</v>
       </c>
       <c r="G71">
-        <v>465488928.6052131</v>
+        <v>19047386780.42</v>
       </c>
       <c r="H71">
-        <v>3955738.469511083</v>
+        <v>222042939.9</v>
       </c>
       <c r="I71">
-        <v>0</v>
+        <v>1758845523.892</v>
       </c>
       <c r="J71">
-        <v>54711.06902621213</v>
+        <v>839559897.548</v>
       </c>
       <c r="K71">
-        <v>1291358.468</v>
+        <v>326675991.672</v>
       </c>
       <c r="L71">
-        <v>44053.16</v>
+        <v>36777056.336</v>
       </c>
       <c r="M71">
-        <v>22429035.556</v>
+        <v>385116208.336</v>
       </c>
       <c r="N71">
-        <v>5345861.166537285</v>
+        <v>5028293939.736</v>
       </c>
       <c r="O71">
-        <v>27774896.72253729</v>
+        <v>5413410148.072001</v>
       </c>
       <c r="P71">
-        <v>493263825.3277504</v>
+        <v>24460796928.492</v>
       </c>
     </row>
     <row r="72">
@@ -4410,12 +4405,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>TA</t>
+          <t>RD</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>TA</t>
+          <t>RD</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -4423,52 +4418,57 @@
           <t>mssf</t>
         </is>
       </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>EU2020_2</t>
+        </is>
+      </c>
       <c r="F72">
-        <v>3776885639.26854</v>
+        <v>13007491012.544</v>
       </c>
       <c r="G72">
-        <v>3118867482.34056</v>
+        <v>7991247439.432</v>
       </c>
       <c r="H72">
-        <v>515627343.856402</v>
+        <v>1031427010.652</v>
       </c>
       <c r="I72">
-        <v>15170574.82</v>
+        <v>3110513.12</v>
       </c>
       <c r="J72">
-        <v>70942998.13957831</v>
+        <v>50777145.608</v>
       </c>
       <c r="K72">
-        <v>14733837.62</v>
+        <v>0</v>
       </c>
       <c r="L72">
-        <v>1486746.076</v>
+        <v>230129200.308</v>
       </c>
       <c r="M72">
-        <v>40047656.416</v>
+        <v>3720575488.952</v>
       </c>
       <c r="N72">
-        <v>617970500.5119803</v>
+        <v>1295668084.16</v>
       </c>
       <c r="O72">
-        <v>658018156.9279803</v>
+        <v>5016243573.112</v>
       </c>
       <c r="P72">
-        <v>3776885639.26854</v>
+        <v>13007491012.544</v>
       </c>
     </row>
     <row r="73">
       <c r="A73">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>INFR</t>
+          <t>TA</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>INFR</t>
+          <t>TA</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -4478,55 +4478,55 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>EU2020_3</t>
+          <t>EU2020_1</t>
         </is>
       </c>
       <c r="F73">
-        <v>290268416.7114286</v>
+        <v>15314323.02257472</v>
       </c>
       <c r="G73">
-        <v>114838837.7342857</v>
+        <v>13915053.37153279</v>
       </c>
       <c r="H73">
-        <v>55314.28571428571</v>
+        <v>952764.5186721447</v>
       </c>
       <c r="I73">
         <v>0</v>
       </c>
       <c r="J73">
-        <v>15042704.3</v>
+        <v>290601.2693666145</v>
       </c>
       <c r="K73">
-        <v>126581951.1428571</v>
+        <v>0</v>
       </c>
       <c r="L73">
-        <v>0</v>
+        <v>24988.87482000001</v>
       </c>
       <c r="M73">
-        <v>33749609.24857143</v>
+        <v>130914.9881831651</v>
       </c>
       <c r="N73">
-        <v>141679969.7285714</v>
+        <v>1268354.662858759</v>
       </c>
       <c r="O73">
-        <v>175429578.9771428</v>
+        <v>1399269.651041924</v>
       </c>
       <c r="P73">
-        <v>290268416.7114286</v>
+        <v>15314323.02257472</v>
       </c>
     </row>
     <row r="74">
       <c r="A74">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>INFR</t>
+          <t>TA</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>INFR</t>
+          <t>TA</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -4534,49 +4534,57 @@
           <t>mssf</t>
         </is>
       </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>EU2020_5</t>
+        </is>
+      </c>
       <c r="F74">
-        <v>984307876.9857142</v>
+        <v>830383819.4010587</v>
       </c>
       <c r="G74">
-        <v>812141173.682857</v>
+        <v>760729709.7370114</v>
       </c>
       <c r="H74">
-        <v>10338457.57142857</v>
+        <v>34742831.07993781</v>
       </c>
       <c r="I74">
-        <v>51193050.60285714</v>
+        <v>0</v>
       </c>
       <c r="J74">
-        <v>723830.8171428571</v>
+        <v>355122.1943623343</v>
       </c>
       <c r="K74">
-        <v>35271355.63714285</v>
+        <v>6542682.236</v>
       </c>
       <c r="L74">
-        <v>3372250.494285714</v>
+        <v>793703.94472</v>
       </c>
       <c r="M74">
-        <v>40507705.14</v>
+        <v>26085721.70102716</v>
       </c>
       <c r="N74">
-        <v>131658998.1628571</v>
+        <v>43568387.96302013</v>
       </c>
       <c r="O74">
-        <v>172166703.3028571</v>
+        <v>69654109.66404729</v>
       </c>
       <c r="P74">
-        <v>984307876.9857142</v>
+        <v>830383819.4010587</v>
       </c>
     </row>
     <row r="75">
+      <c r="A75">
+        <v>2023</v>
+      </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>AIS</t>
+          <t>TA</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>AIS1</t>
+          <t>TA</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -4584,43 +4592,38 @@
           <t>mssf</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>EU2020_2</t>
-        </is>
-      </c>
       <c r="F75">
-        <v>0</v>
+        <v>7223222396.294045</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>5568717059.705028</v>
       </c>
       <c r="H75">
-        <v>0</v>
+        <v>778001618.2627033</v>
       </c>
       <c r="I75">
-        <v>0</v>
+        <v>28536717.58</v>
       </c>
       <c r="J75">
-        <v>0</v>
+        <v>78242681.16418545</v>
       </c>
       <c r="K75">
-        <v>0</v>
+        <v>21020293.192</v>
       </c>
       <c r="L75">
-        <v>0</v>
+        <v>2254676.81446</v>
       </c>
       <c r="M75">
-        <v>0</v>
+        <v>746432608.1196696</v>
       </c>
       <c r="N75">
-        <v>0</v>
+        <v>908072728.4693487</v>
       </c>
       <c r="O75">
-        <v>0</v>
+        <v>1654505336.589018</v>
       </c>
       <c r="P75">
-        <v>0</v>
+        <v>7223222396.294045</v>
       </c>
     </row>
     <row r="76">
@@ -4641,7 +4644,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>EU2020_3</t>
+          <t>EU2020_2</t>
         </is>
       </c>
       <c r="F76">
@@ -4686,7 +4689,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>AIS2</t>
+          <t>AIS1</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -4696,7 +4699,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>EU2020_2</t>
+          <t>EU2020_3</t>
         </is>
       </c>
       <c r="F77">
@@ -4751,7 +4754,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>EU2020_3</t>
+          <t>EU2020_2</t>
         </is>
       </c>
       <c r="F78">
@@ -4806,7 +4809,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>EU2020_5</t>
+          <t>EU2020_3</t>
         </is>
       </c>
       <c r="F79">
@@ -4859,6 +4862,11 @@
           <t>mssf</t>
         </is>
       </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>EU2020_5</t>
+        </is>
+      </c>
       <c r="F80">
         <v>0</v>
       </c>
@@ -4901,17 +4909,12 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>AIS3</t>
+          <t>AIS2</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
           <t>mssf</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>EU2020_2</t>
         </is>
       </c>
       <c r="F81">
@@ -4966,7 +4969,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>EU2020_3</t>
+          <t>EU2020_2</t>
         </is>
       </c>
       <c r="F82">
@@ -5019,6 +5022,11 @@
           <t>mssf</t>
         </is>
       </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>EU2020_3</t>
+        </is>
+      </c>
       <c r="F83">
         <v>0</v>
       </c>
@@ -5061,17 +5069,12 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>AIS4</t>
+          <t>AIS3</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
           <t>mssf</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>EU2020_2</t>
         </is>
       </c>
       <c r="F84">
@@ -5126,7 +5129,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>EU2020_3</t>
+          <t>EU2020_2</t>
         </is>
       </c>
       <c r="F85">
@@ -5181,7 +5184,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>EU2020_5</t>
+          <t>EU2020_3</t>
         </is>
       </c>
       <c r="F86">
@@ -5234,6 +5237,11 @@
           <t>mssf</t>
         </is>
       </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>EU2020_5</t>
+        </is>
+      </c>
       <c r="F87">
         <v>0</v>
       </c>
@@ -5276,17 +5284,12 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>AIS5</t>
+          <t>AIS4</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
           <t>mssf</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>EU2020_2</t>
         </is>
       </c>
       <c r="F88">
@@ -5341,7 +5344,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>EU2020_3</t>
+          <t>EU2020_2</t>
         </is>
       </c>
       <c r="F89">
@@ -5396,7 +5399,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>EU2020_5</t>
+          <t>EU2020_3</t>
         </is>
       </c>
       <c r="F90">
@@ -5449,6 +5452,11 @@
           <t>mssf</t>
         </is>
       </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>EU2020_5</t>
+        </is>
+      </c>
       <c r="F91">
         <v>0</v>
       </c>
@@ -5491,7 +5499,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>AISNA</t>
+          <t>AIS5</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -5536,22 +5544,17 @@
     <row r="93">
       <c r="B93" t="inlineStr">
         <is>
-          <t>HC</t>
+          <t>AIS</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>HC</t>
+          <t>AISNA</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
           <t>mssf</t>
-        </is>
-      </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>EU2020_1</t>
         </is>
       </c>
       <c r="F93">
@@ -5606,7 +5609,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>EU2020_4</t>
+          <t>EU2020_1</t>
         </is>
       </c>
       <c r="F94">
@@ -5661,7 +5664,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>EU2020_5</t>
+          <t>EU2020_4</t>
         </is>
       </c>
       <c r="F95">
@@ -5714,6 +5717,11 @@
           <t>mssf</t>
         </is>
       </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>EU2020_5</t>
+        </is>
+      </c>
       <c r="F96">
         <v>0</v>
       </c>
@@ -5751,22 +5759,17 @@
     <row r="97">
       <c r="B97" t="inlineStr">
         <is>
-          <t>INFR</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>INFR</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
           <t>mssf</t>
-        </is>
-      </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>EU2020_3</t>
         </is>
       </c>
       <c r="F97">
@@ -5821,7 +5824,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>EU2020_5</t>
+          <t>EU2020_3</t>
         </is>
       </c>
       <c r="F98">
@@ -5874,6 +5877,11 @@
           <t>mssf</t>
         </is>
       </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>EU2020_5</t>
+        </is>
+      </c>
       <c r="F99">
         <v>0</v>
       </c>
@@ -5911,22 +5919,17 @@
     <row r="100">
       <c r="B100" t="inlineStr">
         <is>
-          <t>RD</t>
+          <t>INFR</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>RD</t>
+          <t>INFR</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
           <t>mssf</t>
-        </is>
-      </c>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>EU2020_2</t>
         </is>
       </c>
       <c r="F100">
@@ -5966,12 +5969,12 @@
     <row r="101">
       <c r="B101" t="inlineStr">
         <is>
-          <t>TA</t>
+          <t>RD</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>TA</t>
+          <t>RD</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -5981,7 +5984,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>EU2020_1</t>
+          <t>EU2020_2</t>
         </is>
       </c>
       <c r="F101">
@@ -6036,7 +6039,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>EU2020_5</t>
+          <t>EU2020_1</t>
         </is>
       </c>
       <c r="F102">
@@ -6089,6 +6092,11 @@
           <t>mssf</t>
         </is>
       </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>EU2020_5</t>
+        </is>
+      </c>
       <c r="F103">
         <v>0</v>
       </c>
@@ -6120,6 +6128,56 @@
         <v>0</v>
       </c>
       <c r="P103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>TA</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>TA</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>mssf</t>
+        </is>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+      <c r="H104">
+        <v>0</v>
+      </c>
+      <c r="I104">
+        <v>0</v>
+      </c>
+      <c r="J104">
+        <v>0</v>
+      </c>
+      <c r="K104">
+        <v>0</v>
+      </c>
+      <c r="L104">
+        <v>0</v>
+      </c>
+      <c r="M104">
+        <v>0</v>
+      </c>
+      <c r="N104">
+        <v>0</v>
+      </c>
+      <c r="O104">
+        <v>0</v>
+      </c>
+      <c r="P104">
         <v>0</v>
       </c>
     </row>

</xml_diff>